<commit_message>
Update validate_urls, test files, and test.xlsx for improved URL validation
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10913"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spac-43\Dev\Opgaver uge 05 - Krav+PDFdownloader WORK\project\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmbab/Dev/Specialisterne - Opgaver uge 5 (uge 45) Krav+PDFdownloader/Opgaver uge 05 - Krav+PDFdownloader WORK - to improve/project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB3D0965-8533-41EB-9C83-455E5DFC72FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A6FACF5-0C91-3448-8090-A44F7701C2D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2320" windowWidth="18510" windowHeight="9080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9840" yWindow="8880" windowWidth="18520" windowHeight="9080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -46,9 +46,6 @@
     <t>pcartwright@schaefer.com</t>
   </si>
   <si>
-    <t>http://hammes.net/vel-quia-similique-porro-dolor-inventore-omnis-in</t>
-  </si>
-  <si>
     <t>https://www.cassin.com/saepe-optio-sapiente-expedita-saepe-aut</t>
   </si>
   <si>
@@ -61,9 +58,6 @@
     <t>ignacio46@pfeffer.com</t>
   </si>
   <si>
-    <t>http://www.hamill.biz/facilis-ut-facere-non-vel-nobis-et-dignissimos</t>
-  </si>
-  <si>
     <t>https://ferry.com/quo-qui-saepe-dolor-dignissimos-perferendis-suscipit-autem.html</t>
   </si>
   <si>
@@ -79,9 +73,6 @@
     <t>http://www.oreilly.com/impedit-maiores-quia-qui-sed-accusantium</t>
   </si>
   <si>
-    <t>https://ullrich.com/vel-inventore-qui-dolor-dolorem-inventore-iste.html</t>
-  </si>
-  <si>
     <t>Hettinger, Stroman and Bashirian</t>
   </si>
   <si>
@@ -221,6 +212,15 @@
   </si>
   <si>
     <t>https://www.learningcontainer.com/wp-content/uploads/2019/09/sample-pdf-with-images.pdf</t>
+  </si>
+  <si>
+    <t>https://www.bseindia.com/bseplus/AnnualReport/539254/5392540317.pdf</t>
+  </si>
+  <si>
+    <t>https://www.acclimited.com/source/new/ACC-Annual-Report-2016.pdf</t>
+  </si>
+  <si>
+    <t>https://github.com/AI-books/Fundamentals-of-Deep-Learning-EN/blob/317702835956f8d7908329189a05b59a099cc6d9/OReilly.Fundamentals.of.Deep.Learning.2017.5.pdf</t>
   </si>
 </sst>
 </file>
@@ -273,7 +273,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -578,21 +578,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
-      <selection activeCell="AM9" sqref="AM9"/>
+    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
+      <selection activeCell="AM5" sqref="AM5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="40" customWidth="1"/>
-    <col min="3" max="3" width="34.7265625" customWidth="1"/>
-    <col min="4" max="4" width="19.81640625" customWidth="1"/>
+    <col min="3" max="3" width="34.6640625" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="38" max="38" width="97.453125" customWidth="1"/>
-    <col min="39" max="39" width="75.54296875" customWidth="1"/>
+    <col min="38" max="38" width="97.5" customWidth="1"/>
+    <col min="39" max="39" width="75.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -606,15 +606,15 @@
         <v>3</v>
       </c>
       <c r="AL1" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="AM1" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -626,190 +626,190 @@
         <v>6</v>
       </c>
       <c r="AL2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AM2" t="s">
         <v>7</v>
       </c>
-      <c r="AM2" t="s">
+    </row>
+    <row r="3" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AL4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AM4" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>19</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>53</v>
       </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>12</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AM6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>54</v>
       </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>17</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="AL7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AM7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>55</v>
       </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" t="s">
-        <v>21</v>
-      </c>
-      <c r="AL5" t="s">
-        <v>22</v>
-      </c>
-      <c r="AM5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>32</v>
+      </c>
+      <c r="AL8" t="s">
+        <v>33</v>
+      </c>
+      <c r="AM8" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>56</v>
       </c>
-      <c r="B6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" t="s">
-        <v>26</v>
-      </c>
-      <c r="AL6" t="s">
-        <v>27</v>
-      </c>
-      <c r="AM6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL9" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>57</v>
       </c>
-      <c r="B7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL7" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="AM7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" t="s">
+        <v>41</v>
+      </c>
+      <c r="AL10" t="s">
+        <v>42</v>
+      </c>
+      <c r="AM10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>58</v>
       </c>
-      <c r="B8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" t="s">
-        <v>35</v>
-      </c>
-      <c r="AL8" t="s">
-        <v>36</v>
-      </c>
-      <c r="AM8" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>59</v>
-      </c>
-      <c r="B9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" t="s">
-        <v>39</v>
-      </c>
-      <c r="AL9" t="s">
-        <v>40</v>
-      </c>
-      <c r="AM9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>60</v>
-      </c>
-      <c r="B10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="B11" t="s">
         <v>44</v>
       </c>
-      <c r="AL10" t="s">
+      <c r="C11" t="s">
         <v>45</v>
       </c>
-      <c r="AM10" t="s">
+      <c r="D11" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>61</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="AL11" t="s">
         <v>47</v>
       </c>
-      <c r="C11" t="s">
+      <c r="AM11" t="s">
         <v>48</v>
-      </c>
-      <c r="D11" t="s">
-        <v>49</v>
-      </c>
-      <c r="AL11" t="s">
-        <v>50</v>
-      </c>
-      <c r="AM11" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -817,8 +817,11 @@
     <hyperlink ref="AL2" r:id="rId1" xr:uid="{4CC01740-0929-47B4-9BAE-D69DB9E8E7F5}"/>
     <hyperlink ref="AL7" r:id="rId2" xr:uid="{FB968BD1-CF18-4256-988C-F5101ECAFEDD}"/>
     <hyperlink ref="AM8" r:id="rId3" xr:uid="{44CDD5A6-509D-47D4-9DAA-4F4832EDD4BF}"/>
+    <hyperlink ref="AL3" r:id="rId4" xr:uid="{EB22DA33-D588-8B4F-9823-E8501697D28D}"/>
+    <hyperlink ref="AL4" r:id="rId5" xr:uid="{AE88A0CC-863F-DC4F-B980-A3632B85857C}"/>
+    <hyperlink ref="AM4" r:id="rId6" xr:uid="{FFC79EF9-EED3-7645-A176-3C7E7C234DA0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add modified test.xlsx and Metadata2024.xlsx for updated tests
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmbab/Dev/Specialisterne - Opgaver uge 5 (uge 45) Krav+PDFdownloader/Opgaver uge 05 - Krav+PDFdownloader WORK - to improve/project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A6FACF5-0C91-3448-8090-A44F7701C2D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82AD2E8E-ADBB-F04A-9DCC-6B61B4FE4A8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9840" yWindow="8880" windowWidth="18520" windowHeight="9080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30560" windowHeight="15980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -578,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
-      <selection activeCell="AM5" sqref="AM5"/>
+    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
+      <selection activeCell="AM8" sqref="AM8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>